<commit_message>
Updated enduroScreen.xlsx race screen.
</commit_message>
<xml_diff>
--- a/enduroScreen.xlsx
+++ b/enduroScreen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\EnduroComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>m</t>
   </si>
@@ -45,15 +45,6 @@
     <t>p</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Miles to next check</t>
   </si>
   <si>
@@ -208,6 +196,24 @@
   </si>
   <si>
     <t>Clock</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -290,15 +296,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -343,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +624,7 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +650,7 @@
     <col min="20" max="21" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -738,56 +735,48 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="N2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="P2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>9</v>
+      <c r="S2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -795,7 +784,7 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -807,17 +796,14 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="S3" t="s">
+        <v>19</v>
+      </c>
       <c r="T3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="7" t="s">
-        <v>9</v>
+      <c r="U3" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -825,221 +811,238 @@
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="J4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="T4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>22</v>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="V8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="W9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="W10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="V12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="W13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="W14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="V16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="W17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="W18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="V20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="W22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="V24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="W25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1161,7 +1164,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="8"/>
+      <c r="U2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1187,7 +1190,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="9"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1213,7 +1216,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="9"/>
+      <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1239,88 +1242,88 @@
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
-      <c r="U5" s="10"/>
+      <c r="U5" s="9"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Y7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Q8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" t="s">
         <v>44</v>
-      </c>
-      <c r="R10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" t="s">
         <v>45</v>
-      </c>
-      <c r="R11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" t="s">
         <v>46</v>
-      </c>
-      <c r="R12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>